<commit_message>
fix errors on excel file generation; temporary addition of CC for mailer; add env config; fix mail message
</commit_message>
<xml_diff>
--- a/templates/inquiry.xlsx
+++ b/templates/inquiry.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>PRODUCT COST INQUIRY</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>REMARKS</t>
-  </si>
-  <si>
-    <t>pcs</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -781,7 +778,7 @@
   <dimension ref="A1:Z984"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:H11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -979,14 +976,14 @@
         <v>2</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="6"/>
@@ -1015,14 +1012,14 @@
         <v>4</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="6"/>
@@ -1143,14 +1140,12 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
-      <c r="G12" s="22" t="s">
-        <v>11</v>
-      </c>
+      <c r="G12" s="22"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="6"/>
@@ -1175,7 +1170,7 @@
       <c r="A13" s="23"/>
       <c r="B13" s="24"/>
       <c r="C13" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="21"/>
@@ -1205,7 +1200,7 @@
       <c r="A14" s="27"/>
       <c r="B14" s="28"/>
       <c r="C14" s="29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="30"/>
       <c r="E14" s="31"/>

</xml_diff>